<commit_message>
Update issues with API
</commit_message>
<xml_diff>
--- a/static/general/docs/issues.xlsx
+++ b/static/general/docs/issues.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,11 @@
           <t>LAST TRANSACTION</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>SUPPORTED BY</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,12 +471,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023-04-21 06:31:33.872727+00:00</t>
+          <t>2023-06-27</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Hello World</t>
+          <t>Hurted</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Santhosh</t>
         </is>
       </c>
     </row>

</xml_diff>